<commit_message>
🔧 Update trigger-local-update to support both Part and He sync
</commit_message>
<xml_diff>
--- a/assets/Part.xlsx
+++ b/assets/Part.xlsx
@@ -1981,7 +1981,7 @@
         <v>성균관대 CORE400꺼  수리해 온것</v>
       </c>
       <c r="E69" t="str">
-        <v>봉근테스트</v>
+        <v/>
       </c>
       <c r="F69" t="str">
         <v/>
@@ -2530,10 +2530,10 @@
         <v>BOSSI  S1</v>
       </c>
       <c r="D93" t="str">
-        <v>3개</v>
+        <v/>
       </c>
       <c r="E93" t="str">
-        <v>bgtest</v>
+        <v/>
       </c>
       <c r="F93" t="str">
         <v/>

</xml_diff>